<commit_message>
get rid of junk
</commit_message>
<xml_diff>
--- a/sample1.xlsx
+++ b/sample1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17208" windowHeight="10572" firstSheet="8" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17208" windowHeight="10572" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -18,15 +18,16 @@
     <sheet name="locations_groups" sheetId="5" r:id="rId4"/>
     <sheet name="indicators_info" sheetId="7" r:id="rId5"/>
     <sheet name="locations" sheetId="6" r:id="rId6"/>
-    <sheet name="organisation_names" sheetId="9" r:id="rId7"/>
-    <sheet name="organisation_locations" sheetId="10" r:id="rId8"/>
-    <sheet name="organisation_values" sheetId="11" r:id="rId9"/>
-    <sheet name="laboratory_log_actions" sheetId="12" r:id="rId10"/>
-    <sheet name="laboratory_analyzers" sheetId="13" r:id="rId11"/>
+    <sheet name="laboratory_analyzers" sheetId="13" r:id="rId7"/>
+    <sheet name="organisation_names" sheetId="9" r:id="rId8"/>
+    <sheet name="organisation_locations" sheetId="10" r:id="rId9"/>
+    <sheet name="organisation_values" sheetId="11" r:id="rId10"/>
+    <sheet name="laboratory_log_actions" sheetId="12" r:id="rId11"/>
     <sheet name="laboratory_users" sheetId="14" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">indicators_categories!$A$1:$E$400</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">laboratory_analyzers!$A$1:$B$46</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">locations_groups!$A$1:$D$57</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="533">
   <si>
     <t>ion_sum</t>
   </si>
@@ -2837,7 +2838,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -3064,17 +3065,12 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3082,11 +3078,23 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3097,25 +3105,19 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -4319,9 +4321,425 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1" t="s">
+        <v>457</v>
+      </c>
+      <c r="C1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>36</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>37</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>26</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>36</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>37</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>25</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>31</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <f>B11+1</f>
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>8</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <f>B12+1</f>
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>8</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>12</v>
+      </c>
+      <c r="B17">
+        <f>B13+1</f>
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>8</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>13</v>
+      </c>
+      <c r="B18">
+        <f>B14+1</f>
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>8</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <f>B18+1</f>
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>6</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <v>6</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>8</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>6</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>12</v>
+      </c>
+      <c r="B22">
+        <f>B19+1</f>
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <v>5</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>13</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>4</v>
+      </c>
+      <c r="B24">
+        <v>5</v>
+      </c>
+      <c r="C24">
+        <v>5</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>36</v>
+      </c>
+      <c r="B25">
+        <f>B22+1</f>
+        <v>6</v>
+      </c>
+      <c r="C25">
+        <v>7</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>34</v>
+      </c>
+      <c r="B26">
+        <f>B25+1</f>
+        <v>7</v>
+      </c>
+      <c r="C26">
+        <v>9</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>34</v>
+      </c>
+      <c r="B27">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>10</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>12</v>
+      </c>
+      <c r="B28">
+        <f>B26+1</f>
+        <v>8</v>
+      </c>
+      <c r="C28">
+        <v>11</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -4369,78 +4787,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>517</v>
-      </c>
-      <c r="B1" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="76.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="79" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="63" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="109.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="61.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="79" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="80" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" s="80" t="s">
-        <v>522</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4501,7 +4847,7 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:10" ht="42" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="89" t="s">
         <v>54</v>
       </c>
       <c r="B1" s="22" t="s">
@@ -4510,14 +4856,14 @@
       <c r="C1" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="86" t="s">
+      <c r="D1" s="85" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="87"/>
-      <c r="F1" s="86" t="s">
+      <c r="E1" s="86"/>
+      <c r="F1" s="85" t="s">
         <v>58</v>
       </c>
-      <c r="G1" s="87"/>
+      <c r="G1" s="86"/>
       <c r="H1" s="23" t="s">
         <v>59</v>
       </c>
@@ -4526,7 +4872,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="42" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="94"/>
+      <c r="A2" s="90"/>
       <c r="B2" s="24" t="s">
         <v>61</v>
       </c>
@@ -4553,7 +4899,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="45" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="93" t="s">
+      <c r="A3" s="89" t="s">
         <v>62</v>
       </c>
       <c r="B3" s="26" t="s">
@@ -4582,7 +4928,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="94"/>
+      <c r="A4" s="90"/>
       <c r="B4" s="26" t="s">
         <v>71</v>
       </c>
@@ -4609,7 +4955,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="96" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="93" t="s">
+      <c r="A5" s="89" t="s">
         <v>78</v>
       </c>
       <c r="B5" s="26" t="s">
@@ -4638,7 +4984,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="94"/>
+      <c r="A6" s="90"/>
       <c r="B6" s="26" t="s">
         <v>71</v>
       </c>
@@ -4665,7 +5011,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="45" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="93" t="s">
+      <c r="A7" s="89" t="s">
         <v>93</v>
       </c>
       <c r="B7" s="26" t="s">
@@ -4694,7 +5040,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="94"/>
+      <c r="A8" s="90"/>
       <c r="B8" s="26" t="s">
         <v>71</v>
       </c>
@@ -4721,7 +5067,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="45" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="93" t="s">
+      <c r="A9" s="89" t="s">
         <v>106</v>
       </c>
       <c r="B9" s="26" t="s">
@@ -4750,7 +5096,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="94"/>
+      <c r="A10" s="90"/>
       <c r="B10" s="26" t="s">
         <v>71</v>
       </c>
@@ -4777,7 +5123,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="42" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="93" t="s">
+      <c r="A11" s="89" t="s">
         <v>156</v>
       </c>
       <c r="B11" s="22" t="s">
@@ -4786,24 +5132,24 @@
       <c r="C11" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="86" t="s">
+      <c r="D11" s="85" t="s">
         <v>57</v>
       </c>
-      <c r="E11" s="87"/>
-      <c r="F11" s="86" t="s">
+      <c r="E11" s="86"/>
+      <c r="F11" s="85" t="s">
         <v>58</v>
       </c>
-      <c r="G11" s="87"/>
+      <c r="G11" s="86"/>
       <c r="H11" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="I11" s="86" t="s">
+      <c r="I11" s="85" t="s">
         <v>60</v>
       </c>
-      <c r="J11" s="87"/>
+      <c r="J11" s="86"/>
     </row>
     <row r="12" spans="1:10" ht="42" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="94"/>
+      <c r="A12" s="90"/>
       <c r="B12" s="24" t="s">
         <v>61</v>
       </c>
@@ -4831,10 +5177,10 @@
       <c r="J12" s="43"/>
     </row>
     <row r="13" spans="1:10" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="95" t="s">
+      <c r="A13" s="87" t="s">
         <v>157</v>
       </c>
-      <c r="B13" s="96"/>
+      <c r="B13" s="88"/>
       <c r="C13" s="13" t="s">
         <v>158</v>
       </c>
@@ -4859,10 +5205,10 @@
       <c r="J13" s="47"/>
     </row>
     <row r="14" spans="1:10" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="95" t="s">
+      <c r="A14" s="87" t="s">
         <v>162</v>
       </c>
-      <c r="B14" s="96"/>
+      <c r="B14" s="88"/>
       <c r="C14" s="25" t="s">
         <v>163</v>
       </c>
@@ -4887,10 +5233,10 @@
       <c r="J14" s="47"/>
     </row>
     <row r="15" spans="1:10" ht="41.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="95" t="s">
+      <c r="A15" s="87" t="s">
         <v>169</v>
       </c>
-      <c r="B15" s="96"/>
+      <c r="B15" s="88"/>
       <c r="C15" s="25" t="s">
         <v>170</v>
       </c>
@@ -4915,10 +5261,10 @@
       <c r="J15" s="47"/>
     </row>
     <row r="16" spans="1:10" ht="41.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="95" t="s">
+      <c r="A16" s="87" t="s">
         <v>175</v>
       </c>
-      <c r="B16" s="96"/>
+      <c r="B16" s="88"/>
       <c r="C16" s="25" t="s">
         <v>79</v>
       </c>
@@ -4943,7 +5289,7 @@
       <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10" ht="41.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="93" t="s">
+      <c r="A17" s="89" t="s">
         <v>156</v>
       </c>
       <c r="B17" s="22" t="s">
@@ -4952,14 +5298,14 @@
       <c r="C17" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="D17" s="86" t="s">
+      <c r="D17" s="85" t="s">
         <v>57</v>
       </c>
-      <c r="E17" s="87"/>
-      <c r="F17" s="86" t="s">
+      <c r="E17" s="86"/>
+      <c r="F17" s="85" t="s">
         <v>58</v>
       </c>
-      <c r="G17" s="87"/>
+      <c r="G17" s="86"/>
       <c r="H17" s="32" t="s">
         <v>59</v>
       </c>
@@ -4969,7 +5315,7 @@
       <c r="J17" s="54"/>
     </row>
     <row r="18" spans="1:10" ht="41.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="94"/>
+      <c r="A18" s="90"/>
       <c r="B18" s="24" t="s">
         <v>61</v>
       </c>
@@ -4997,10 +5343,10 @@
       <c r="J18" s="54"/>
     </row>
     <row r="19" spans="1:10" ht="41.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="95" t="s">
+      <c r="A19" s="87" t="s">
         <v>119</v>
       </c>
-      <c r="B19" s="96"/>
+      <c r="B19" s="88"/>
       <c r="C19" s="25" t="s">
         <v>158</v>
       </c>
@@ -5025,10 +5371,10 @@
       <c r="J19" s="54"/>
     </row>
     <row r="20" spans="1:10" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="95" t="s">
+      <c r="A20" s="87" t="s">
         <v>120</v>
       </c>
-      <c r="B20" s="96"/>
+      <c r="B20" s="88"/>
       <c r="C20" s="25" t="s">
         <v>163</v>
       </c>
@@ -5053,10 +5399,10 @@
       <c r="J20" s="54"/>
     </row>
     <row r="21" spans="1:10" ht="41.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="95" t="s">
+      <c r="A21" s="87" t="s">
         <v>121</v>
       </c>
-      <c r="B21" s="96"/>
+      <c r="B21" s="88"/>
       <c r="C21" s="25" t="s">
         <v>301</v>
       </c>
@@ -5081,10 +5427,10 @@
       <c r="J21" s="54"/>
     </row>
     <row r="22" spans="1:10" ht="55.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="95" t="s">
+      <c r="A22" s="87" t="s">
         <v>122</v>
       </c>
-      <c r="B22" s="96"/>
+      <c r="B22" s="88"/>
       <c r="C22" s="25" t="s">
         <v>308</v>
       </c>
@@ -5151,14 +5497,14 @@
       <c r="B26" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="86" t="s">
+      <c r="C26" s="85" t="s">
         <v>57</v>
       </c>
-      <c r="D26" s="87"/>
-      <c r="E26" s="86" t="s">
+      <c r="D26" s="86"/>
+      <c r="E26" s="85" t="s">
         <v>58</v>
       </c>
-      <c r="F26" s="87"/>
+      <c r="F26" s="86"/>
       <c r="G26" s="32" t="s">
         <v>59</v>
       </c>
@@ -5170,25 +5516,25 @@
       <c r="A27" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="B27" s="82">
+      <c r="B27" s="91">
         <v>1</v>
       </c>
-      <c r="C27" s="82">
+      <c r="C27" s="91">
         <v>2</v>
       </c>
-      <c r="D27" s="82">
+      <c r="D27" s="91">
         <v>3</v>
       </c>
-      <c r="E27" s="82">
+      <c r="E27" s="91">
         <v>4</v>
       </c>
-      <c r="F27" s="82">
+      <c r="F27" s="91">
         <v>5</v>
       </c>
-      <c r="G27" s="82">
+      <c r="G27" s="91">
         <v>6</v>
       </c>
-      <c r="H27" s="82">
+      <c r="H27" s="91">
         <v>7</v>
       </c>
     </row>
@@ -5196,25 +5542,25 @@
       <c r="A28" s="31" t="s">
         <v>177</v>
       </c>
-      <c r="B28" s="83"/>
-      <c r="C28" s="83"/>
-      <c r="D28" s="83"/>
-      <c r="E28" s="83"/>
-      <c r="F28" s="83"/>
-      <c r="G28" s="83"/>
-      <c r="H28" s="83"/>
+      <c r="B28" s="92"/>
+      <c r="C28" s="92"/>
+      <c r="D28" s="92"/>
+      <c r="E28" s="92"/>
+      <c r="F28" s="92"/>
+      <c r="G28" s="92"/>
+      <c r="H28" s="92"/>
     </row>
     <row r="29" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="90" t="s">
+      <c r="A29" s="93" t="s">
         <v>49</v>
       </c>
-      <c r="B29" s="91"/>
-      <c r="C29" s="91"/>
-      <c r="D29" s="91"/>
-      <c r="E29" s="91"/>
-      <c r="F29" s="91"/>
-      <c r="G29" s="91"/>
-      <c r="H29" s="92"/>
+      <c r="B29" s="94"/>
+      <c r="C29" s="94"/>
+      <c r="D29" s="94"/>
+      <c r="E29" s="94"/>
+      <c r="F29" s="94"/>
+      <c r="G29" s="94"/>
+      <c r="H29" s="95"/>
     </row>
     <row r="30" spans="1:10" ht="73.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="31" t="s">
@@ -5295,16 +5641,16 @@
       </c>
     </row>
     <row r="33" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="90" t="s">
+      <c r="A33" s="93" t="s">
         <v>50</v>
       </c>
-      <c r="B33" s="91"/>
-      <c r="C33" s="91"/>
-      <c r="D33" s="91"/>
-      <c r="E33" s="91"/>
-      <c r="F33" s="91"/>
-      <c r="G33" s="91"/>
-      <c r="H33" s="92"/>
+      <c r="B33" s="94"/>
+      <c r="C33" s="94"/>
+      <c r="D33" s="94"/>
+      <c r="E33" s="94"/>
+      <c r="F33" s="94"/>
+      <c r="G33" s="94"/>
+      <c r="H33" s="95"/>
     </row>
     <row r="34" spans="1:8" ht="45" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="31" t="s">
@@ -5385,16 +5731,16 @@
       </c>
     </row>
     <row r="37" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="90" t="s">
+      <c r="A37" s="93" t="s">
         <v>51</v>
       </c>
-      <c r="B37" s="91"/>
-      <c r="C37" s="91"/>
-      <c r="D37" s="91"/>
-      <c r="E37" s="91"/>
-      <c r="F37" s="91"/>
-      <c r="G37" s="91"/>
-      <c r="H37" s="92"/>
+      <c r="B37" s="94"/>
+      <c r="C37" s="94"/>
+      <c r="D37" s="94"/>
+      <c r="E37" s="94"/>
+      <c r="F37" s="94"/>
+      <c r="G37" s="94"/>
+      <c r="H37" s="95"/>
     </row>
     <row r="38" spans="1:8" ht="58.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="31" t="s">
@@ -5501,16 +5847,16 @@
       </c>
     </row>
     <row r="42" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="90" t="s">
+      <c r="A42" s="93" t="s">
         <v>52</v>
       </c>
-      <c r="B42" s="91"/>
-      <c r="C42" s="91"/>
-      <c r="D42" s="91"/>
-      <c r="E42" s="91"/>
-      <c r="F42" s="91"/>
-      <c r="G42" s="91"/>
-      <c r="H42" s="92"/>
+      <c r="B42" s="94"/>
+      <c r="C42" s="94"/>
+      <c r="D42" s="94"/>
+      <c r="E42" s="94"/>
+      <c r="F42" s="94"/>
+      <c r="G42" s="94"/>
+      <c r="H42" s="95"/>
     </row>
     <row r="43" spans="1:8" ht="45" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="31" t="s">
@@ -5565,16 +5911,16 @@
       </c>
     </row>
     <row r="45" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="90" t="s">
+      <c r="A45" s="93" t="s">
         <v>53</v>
       </c>
-      <c r="B45" s="91"/>
-      <c r="C45" s="91"/>
-      <c r="D45" s="91"/>
-      <c r="E45" s="91"/>
-      <c r="F45" s="91"/>
-      <c r="G45" s="91"/>
-      <c r="H45" s="92"/>
+      <c r="B45" s="94"/>
+      <c r="C45" s="94"/>
+      <c r="D45" s="94"/>
+      <c r="E45" s="94"/>
+      <c r="F45" s="94"/>
+      <c r="G45" s="94"/>
+      <c r="H45" s="95"/>
     </row>
     <row r="46" spans="1:8" ht="45" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="52" t="s">
@@ -5687,14 +6033,14 @@
       <c r="B50" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="C50" s="84" t="s">
+      <c r="C50" s="96" t="s">
         <v>57</v>
       </c>
-      <c r="D50" s="85"/>
-      <c r="E50" s="86" t="s">
+      <c r="D50" s="97"/>
+      <c r="E50" s="85" t="s">
         <v>318</v>
       </c>
-      <c r="F50" s="87"/>
+      <c r="F50" s="86"/>
       <c r="G50" s="32" t="s">
         <v>59</v>
       </c>
@@ -5706,25 +6052,25 @@
       <c r="A51" s="50" t="s">
         <v>319</v>
       </c>
-      <c r="B51" s="88">
+      <c r="B51" s="98">
         <v>1</v>
       </c>
-      <c r="C51" s="82">
+      <c r="C51" s="91">
         <v>2</v>
       </c>
-      <c r="D51" s="82">
+      <c r="D51" s="91">
         <v>3</v>
       </c>
-      <c r="E51" s="82">
+      <c r="E51" s="91">
         <v>4</v>
       </c>
-      <c r="F51" s="82">
+      <c r="F51" s="91">
         <v>5</v>
       </c>
-      <c r="G51" s="82">
+      <c r="G51" s="91">
         <v>6</v>
       </c>
-      <c r="H51" s="82">
+      <c r="H51" s="91">
         <v>7</v>
       </c>
     </row>
@@ -5732,13 +6078,13 @@
       <c r="A52" s="31" t="s">
         <v>177</v>
       </c>
-      <c r="B52" s="89"/>
-      <c r="C52" s="83"/>
-      <c r="D52" s="83"/>
-      <c r="E52" s="83"/>
-      <c r="F52" s="83"/>
-      <c r="G52" s="83"/>
-      <c r="H52" s="83"/>
+      <c r="B52" s="99"/>
+      <c r="C52" s="92"/>
+      <c r="D52" s="92"/>
+      <c r="E52" s="92"/>
+      <c r="F52" s="92"/>
+      <c r="G52" s="92"/>
+      <c r="H52" s="92"/>
     </row>
     <row r="53" spans="1:8" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="31" t="s">
@@ -6392,26 +6738,15 @@
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G51:G52"/>
+    <mergeCell ref="H51:H52"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="F51:F52"/>
     <mergeCell ref="A45:H45"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="D17:E17"/>
@@ -6428,15 +6763,26 @@
     <mergeCell ref="A29:H29"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G51:G52"/>
-    <mergeCell ref="H51:H52"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -13372,7 +13718,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="98" t="s">
+      <c r="A7" s="83" t="s">
         <v>532</v>
       </c>
       <c r="B7">
@@ -13401,7 +13747,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="98" t="s">
+      <c r="A9" s="83" t="s">
         <v>532</v>
       </c>
       <c r="B9">
@@ -13462,7 +13808,7 @@
       <c r="A13" s="77" t="s">
         <v>532</v>
       </c>
-      <c r="B13" s="99">
+      <c r="B13" s="84">
         <v>11</v>
       </c>
       <c r="C13" s="66" t="s">
@@ -13516,7 +13862,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="98" t="s">
+      <c r="A17" s="83" t="s">
         <v>532</v>
       </c>
       <c r="B17">
@@ -13545,7 +13891,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="98" t="s">
+      <c r="A19" s="83" t="s">
         <v>532</v>
       </c>
       <c r="B19">
@@ -13588,7 +13934,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="98" t="s">
+      <c r="A22" s="83" t="s">
         <v>532</v>
       </c>
       <c r="B22">
@@ -13617,7 +13963,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A24" s="98" t="s">
+      <c r="A24" s="83" t="s">
         <v>532</v>
       </c>
       <c r="B24">
@@ -13646,7 +13992,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="98" t="s">
+      <c r="A26" s="83" t="s">
         <v>532</v>
       </c>
       <c r="B26">
@@ -13703,7 +14049,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="98" t="s">
+      <c r="A30" s="83" t="s">
         <v>532</v>
       </c>
       <c r="B30">
@@ -13746,7 +14092,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A33" s="98" t="s">
+      <c r="A33" s="83" t="s">
         <v>532</v>
       </c>
       <c r="B33">
@@ -13804,7 +14150,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="98" t="s">
+      <c r="A37" s="83" t="s">
         <v>532</v>
       </c>
       <c r="B37">
@@ -13847,7 +14193,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="98" t="s">
+      <c r="A40" s="83" t="s">
         <v>532</v>
       </c>
       <c r="B40">
@@ -13862,7 +14208,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A41" s="97" t="s">
+      <c r="A41" s="82" t="s">
         <v>129</v>
       </c>
       <c r="B41" s="27">
@@ -13890,7 +14236,7 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="98" t="s">
+      <c r="A43" s="83" t="s">
         <v>532</v>
       </c>
       <c r="B43">
@@ -13933,7 +14279,7 @@
       </c>
     </row>
     <row r="46" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="98" t="s">
+      <c r="A46" s="83" t="s">
         <v>532</v>
       </c>
       <c r="B46">
@@ -13976,7 +14322,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A49" s="98" t="s">
+      <c r="A49" s="83" t="s">
         <v>532</v>
       </c>
       <c r="B49">
@@ -14033,7 +14379,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A53" s="98" t="s">
+      <c r="A53" s="83" t="s">
         <v>532</v>
       </c>
       <c r="B53">
@@ -14116,10 +14462,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F998"/>
+  <dimension ref="A1:G998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14127,9 +14473,10 @@
     <col min="1" max="1" width="16.44140625" customWidth="1"/>
     <col min="2" max="2" width="8.88671875" style="40"/>
     <col min="6" max="6" width="21.33203125" customWidth="1"/>
+    <col min="7" max="7" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>150</v>
       </c>
@@ -14148,8 +14495,11 @@
       <c r="F1" s="19" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="49.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="49.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -14168,8 +14518,11 @@
       <c r="F2" t="s">
         <v>479</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -14189,8 +14542,12 @@
       <c r="F3" t="s">
         <v>479</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="31.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G3">
+        <f>G2+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="31.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4">
         <f t="shared" ref="A4:A46" si="0">A3+1</f>
         <v>3</v>
@@ -14210,8 +14567,12 @@
       <c r="F4" s="62" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G4">
+        <f t="shared" ref="G4:G46" si="1">G3+1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -14231,8 +14592,12 @@
       <c r="F5" s="62" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="28.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="28.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -14252,8 +14617,12 @@
       <c r="F6" s="62" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -14273,8 +14642,12 @@
       <c r="F7" s="62" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -14294,8 +14667,12 @@
       <c r="F8" s="62" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="34.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="34.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -14315,8 +14692,12 @@
       <c r="F9" s="62" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -14336,8 +14717,12 @@
       <c r="F10" s="62" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -14357,8 +14742,12 @@
       <c r="F11" s="62" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -14378,8 +14767,12 @@
       <c r="F12" s="62" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -14399,8 +14792,12 @@
       <c r="F13" s="62" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -14420,8 +14817,12 @@
       <c r="F14" s="62" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -14441,8 +14842,12 @@
       <c r="F15" s="62" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="31.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="31.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -14462,8 +14867,12 @@
       <c r="F16" s="62" t="s">
         <v>485</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -14483,8 +14892,12 @@
       <c r="F17" s="62" t="s">
         <v>485</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -14504,8 +14917,12 @@
       <c r="F18" s="62" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -14525,8 +14942,12 @@
       <c r="F19" s="62" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -14546,8 +14967,12 @@
       <c r="F20" s="62" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -14567,8 +14992,12 @@
       <c r="F21" s="62" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -14586,8 +15015,12 @@
         <v>9</v>
       </c>
       <c r="F22" s="21"/>
-    </row>
-    <row r="23" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -14605,8 +15038,12 @@
         <v>9</v>
       </c>
       <c r="F23" s="21"/>
-    </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -14624,8 +15061,12 @@
         <v>9</v>
       </c>
       <c r="F24" s="21"/>
-    </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -14643,8 +15084,12 @@
         <v>9</v>
       </c>
       <c r="F25" s="21"/>
-    </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G25">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -14662,8 +15107,12 @@
         <v>9</v>
       </c>
       <c r="F26" s="21"/>
-    </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G26">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -14681,8 +15130,12 @@
         <v>9</v>
       </c>
       <c r="F27" s="21"/>
-    </row>
-    <row r="28" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G27">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -14700,8 +15153,12 @@
         <v>9</v>
       </c>
       <c r="F28" s="21"/>
-    </row>
-    <row r="29" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -14719,8 +15176,12 @@
         <v>9</v>
       </c>
       <c r="F29" s="21"/>
-    </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G29">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -14738,8 +15199,12 @@
         <v>9</v>
       </c>
       <c r="F30" s="21"/>
-    </row>
-    <row r="31" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G30">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -14757,8 +15222,12 @@
         <v>9</v>
       </c>
       <c r="F31" s="21"/>
-    </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G31">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -14776,8 +15245,12 @@
         <v>9</v>
       </c>
       <c r="F32" s="21"/>
-    </row>
-    <row r="33" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G32">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -14795,8 +15268,12 @@
         <v>9</v>
       </c>
       <c r="F33" s="21"/>
-    </row>
-    <row r="34" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G33">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -14814,8 +15291,12 @@
         <v>9</v>
       </c>
       <c r="F34" s="21"/>
-    </row>
-    <row r="35" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G34">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -14833,8 +15314,12 @@
         <v>9</v>
       </c>
       <c r="F35" s="21"/>
-    </row>
-    <row r="36" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G35">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -14852,8 +15337,12 @@
         <v>9</v>
       </c>
       <c r="F36" s="21"/>
-    </row>
-    <row r="37" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G36">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -14871,8 +15360,12 @@
         <v>9</v>
       </c>
       <c r="F37" s="21"/>
-    </row>
-    <row r="38" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G37">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -14890,8 +15383,12 @@
         <v>9</v>
       </c>
       <c r="F38" s="21"/>
-    </row>
-    <row r="39" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G38">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -14909,8 +15406,12 @@
         <v>9</v>
       </c>
       <c r="F39" s="21"/>
-    </row>
-    <row r="40" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G39">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -14928,8 +15429,12 @@
         <v>9</v>
       </c>
       <c r="F40" s="21"/>
-    </row>
-    <row r="41" spans="1:6" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G40">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -14947,8 +15452,12 @@
         <v>9</v>
       </c>
       <c r="F41" s="21"/>
-    </row>
-    <row r="42" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G41">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -14966,8 +15475,12 @@
         <v>9</v>
       </c>
       <c r="F42" s="21"/>
-    </row>
-    <row r="43" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G42">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -14985,8 +15498,12 @@
         <v>9</v>
       </c>
       <c r="F43" s="21"/>
-    </row>
-    <row r="44" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G43">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -15004,8 +15521,12 @@
         <v>9</v>
       </c>
       <c r="F44" s="21"/>
-    </row>
-    <row r="45" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G44">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -15023,8 +15544,12 @@
         <v>9</v>
       </c>
       <c r="F45" s="21"/>
-    </row>
-    <row r="46" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G45">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -15042,14 +15567,18 @@
         <v>9</v>
       </c>
       <c r="F46" s="21"/>
-    </row>
-    <row r="47" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G46">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B47" s="39"/>
       <c r="D47" s="21"/>
       <c r="E47" s="21"/>
       <c r="F47" s="21"/>
     </row>
-    <row r="48" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B48" s="39"/>
       <c r="D48" s="21"/>
       <c r="E48" s="21"/>
@@ -20955,6 +21484,532 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>517</v>
+      </c>
+      <c r="B1" t="s">
+        <v>518</v>
+      </c>
+      <c r="C1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="76.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="79" t="s">
+        <v>519</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="C3" s="100">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="109.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="61.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="79" t="s">
+        <v>524</v>
+      </c>
+      <c r="C5" s="4">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="80" t="s">
+        <v>521</v>
+      </c>
+      <c r="C6" s="4">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="31.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="80" t="s">
+        <v>522</v>
+      </c>
+      <c r="C7" s="4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="109.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="C8" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="109.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="C9" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="109.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="C10" s="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="109.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="C11" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="76.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" s="79" t="s">
+        <v>519</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="76.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" s="79" t="s">
+        <v>519</v>
+      </c>
+      <c r="C13" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="76.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" s="79" t="s">
+        <v>519</v>
+      </c>
+      <c r="C14" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="76.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" s="79" t="s">
+        <v>519</v>
+      </c>
+      <c r="C15" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="76.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" s="79" t="s">
+        <v>519</v>
+      </c>
+      <c r="C16" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="76.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" s="79" t="s">
+        <v>519</v>
+      </c>
+      <c r="C17" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="76.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" s="79" t="s">
+        <v>519</v>
+      </c>
+      <c r="C18" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="76.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" s="79" t="s">
+        <v>519</v>
+      </c>
+      <c r="C19" s="100">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20" s="80" t="s">
+        <v>521</v>
+      </c>
+      <c r="C20" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>5</v>
+      </c>
+      <c r="B21" s="80" t="s">
+        <v>521</v>
+      </c>
+      <c r="C21" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>5</v>
+      </c>
+      <c r="B22" s="80" t="s">
+        <v>521</v>
+      </c>
+      <c r="C22" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>5</v>
+      </c>
+      <c r="B23" s="80" t="s">
+        <v>521</v>
+      </c>
+      <c r="C23" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24" s="80" t="s">
+        <v>521</v>
+      </c>
+      <c r="C24" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>5</v>
+      </c>
+      <c r="B25" s="80" t="s">
+        <v>521</v>
+      </c>
+      <c r="C25" s="4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>5</v>
+      </c>
+      <c r="B26" s="80" t="s">
+        <v>521</v>
+      </c>
+      <c r="C26" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>5</v>
+      </c>
+      <c r="B27" s="80" t="s">
+        <v>521</v>
+      </c>
+      <c r="C27" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>5</v>
+      </c>
+      <c r="B28" s="80" t="s">
+        <v>521</v>
+      </c>
+      <c r="C28" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>5</v>
+      </c>
+      <c r="B29" s="80" t="s">
+        <v>521</v>
+      </c>
+      <c r="C29" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>5</v>
+      </c>
+      <c r="B30" s="80" t="s">
+        <v>521</v>
+      </c>
+      <c r="C30" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>5</v>
+      </c>
+      <c r="B31" s="80" t="s">
+        <v>521</v>
+      </c>
+      <c r="C31" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>5</v>
+      </c>
+      <c r="B32" s="80" t="s">
+        <v>521</v>
+      </c>
+      <c r="C32" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>5</v>
+      </c>
+      <c r="B33" s="80" t="s">
+        <v>521</v>
+      </c>
+      <c r="C33" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>5</v>
+      </c>
+      <c r="B34" s="80" t="s">
+        <v>521</v>
+      </c>
+      <c r="C34" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>5</v>
+      </c>
+      <c r="B35" s="80" t="s">
+        <v>521</v>
+      </c>
+      <c r="C35" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>5</v>
+      </c>
+      <c r="B36" s="80" t="s">
+        <v>521</v>
+      </c>
+      <c r="C36" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>5</v>
+      </c>
+      <c r="B37" s="80" t="s">
+        <v>521</v>
+      </c>
+      <c r="C37" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>5</v>
+      </c>
+      <c r="B38" s="80" t="s">
+        <v>521</v>
+      </c>
+      <c r="C38" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>5</v>
+      </c>
+      <c r="B39" s="80" t="s">
+        <v>521</v>
+      </c>
+      <c r="C39" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>5</v>
+      </c>
+      <c r="B40" s="80" t="s">
+        <v>521</v>
+      </c>
+      <c r="C40" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>5</v>
+      </c>
+      <c r="B41" s="80" t="s">
+        <v>521</v>
+      </c>
+      <c r="C41" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>5</v>
+      </c>
+      <c r="B42" s="80" t="s">
+        <v>521</v>
+      </c>
+      <c r="C42" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>5</v>
+      </c>
+      <c r="B43" s="80" t="s">
+        <v>521</v>
+      </c>
+      <c r="C43" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>5</v>
+      </c>
+      <c r="B44" s="80" t="s">
+        <v>521</v>
+      </c>
+      <c r="C44" s="100">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="61.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>4</v>
+      </c>
+      <c r="B45" s="79" t="s">
+        <v>524</v>
+      </c>
+      <c r="C45" s="4">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="61.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>4</v>
+      </c>
+      <c r="B46" s="79" t="s">
+        <v>524</v>
+      </c>
+      <c r="C46" s="4">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B46"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -21080,7 +22135,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
@@ -21199,420 +22254,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B1" t="s">
-        <v>457</v>
-      </c>
-      <c r="C1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D1" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>8</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>9</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>4</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>4</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>36</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>37</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-      <c r="D9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>26</v>
-      </c>
-      <c r="B10">
-        <v>2</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>36</v>
-      </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="D11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>37</v>
-      </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>25</v>
-      </c>
-      <c r="B13">
-        <v>2</v>
-      </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="D13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>31</v>
-      </c>
-      <c r="B14">
-        <v>2</v>
-      </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="D14">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>18</v>
-      </c>
-      <c r="B15">
-        <f>B11+1</f>
-        <v>3</v>
-      </c>
-      <c r="C15">
-        <v>8</v>
-      </c>
-      <c r="D15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16">
-        <f>B12+1</f>
-        <v>3</v>
-      </c>
-      <c r="C16">
-        <v>8</v>
-      </c>
-      <c r="D16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>12</v>
-      </c>
-      <c r="B17">
-        <f>B13+1</f>
-        <v>3</v>
-      </c>
-      <c r="C17">
-        <v>8</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>13</v>
-      </c>
-      <c r="B18">
-        <f>B14+1</f>
-        <v>3</v>
-      </c>
-      <c r="C18">
-        <v>8</v>
-      </c>
-      <c r="D18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>4</v>
-      </c>
-      <c r="B19">
-        <f>B18+1</f>
-        <v>4</v>
-      </c>
-      <c r="C19">
-        <v>6</v>
-      </c>
-      <c r="D19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>17</v>
-      </c>
-      <c r="B20">
-        <v>4</v>
-      </c>
-      <c r="C20">
-        <v>6</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>8</v>
-      </c>
-      <c r="B21">
-        <v>4</v>
-      </c>
-      <c r="C21">
-        <v>6</v>
-      </c>
-      <c r="D21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>12</v>
-      </c>
-      <c r="B22">
-        <f>B19+1</f>
-        <v>5</v>
-      </c>
-      <c r="C22">
-        <v>5</v>
-      </c>
-      <c r="D22">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>13</v>
-      </c>
-      <c r="B23">
-        <v>5</v>
-      </c>
-      <c r="C23">
-        <v>5</v>
-      </c>
-      <c r="D23">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>4</v>
-      </c>
-      <c r="B24">
-        <v>5</v>
-      </c>
-      <c r="C24">
-        <v>5</v>
-      </c>
-      <c r="D24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>36</v>
-      </c>
-      <c r="B25">
-        <f>B22+1</f>
-        <v>6</v>
-      </c>
-      <c r="C25">
-        <v>7</v>
-      </c>
-      <c r="D25">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>34</v>
-      </c>
-      <c r="B26">
-        <f>B25+1</f>
-        <v>7</v>
-      </c>
-      <c r="C26">
-        <v>9</v>
-      </c>
-      <c r="D26">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>34</v>
-      </c>
-      <c r="B27">
-        <v>8</v>
-      </c>
-      <c r="C27">
-        <v>10</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <v>12</v>
-      </c>
-      <c r="B28">
-        <f>B26+1</f>
-        <v>8</v>
-      </c>
-      <c r="C28">
-        <v>11</v>
-      </c>
-      <c r="D28">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>